<commit_message>
Resending emails to unknown senders works fine
</commit_message>
<xml_diff>
--- a/kontakty.xlsx
+++ b/kontakty.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Piotrek\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Piotrek\Desktop\DankaPracaDomowa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C89A2B6-DD1E-4A76-BC0E-89D7AC25BE3A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39DA696F-1E30-44DB-B9CE-1A332A9FE0CB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="41">
   <si>
     <t>ID</t>
   </si>
@@ -143,15 +143,6 @@
   </si>
   <si>
     <t>Marlena Łabędzka &lt;m.labedzka@hr.info.pl&gt;</t>
-  </si>
-  <si>
-    <t>Magdalena Bawolak &lt;m.bawolak@hr.info.pl&gt;</t>
-  </si>
-  <si>
-    <t> HRS Projekt Sp.z o.o.</t>
-  </si>
-  <si>
-    <t>Sylwia Matejek &lt;s.matejek@hr.info.pl&gt;</t>
   </si>
 </sst>
 </file>
@@ -565,14 +556,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="43.28515625" customWidth="1"/>
-    <col min="3" max="3" width="29.28515625" customWidth="1"/>
+    <col min="3" max="3" width="39" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -923,7 +914,7 @@
       <c r="B32" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C32" s="3" t="s">
         <v>34</v>
       </c>
     </row>
@@ -971,28 +962,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="2">
-        <v>36</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="2">
-        <v>37</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
+    <row r="38" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" display="mailto:z.abramowicz@op.pl" xr:uid="{DD45DCBE-7A22-40B5-8751-8F965EE828D1}"/>
@@ -1029,10 +999,8 @@
     <hyperlink ref="C34" r:id="rId32" display="mailto:lescap9695@wp.pl" xr:uid="{77C52E25-5646-4C6F-9E7F-BFD6C11A6646}"/>
     <hyperlink ref="C35" r:id="rId33" display="mailto:d.husiatynski@danka.com.pl" xr:uid="{C34B628C-5961-4429-B54D-ED7F3A11AEF7}"/>
     <hyperlink ref="C36" r:id="rId34" display="mailto:m.labedzka@hr.info.pl" xr:uid="{36CB5E3E-23AD-415B-AA73-47DAD293CFBB}"/>
-    <hyperlink ref="C37" r:id="rId35" display="mailto:m.bawolak@hr.info.pl" xr:uid="{062FEEFE-E3DF-4111-9FB4-78D60A35282E}"/>
-    <hyperlink ref="C38" r:id="rId36" display="mailto:s.matejek@hr.info.pl" xr:uid="{A80A9001-12F6-4C7D-BC21-82A543DD966E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId37"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId35"/>
 </worksheet>
 </file>
</xml_diff>